<commit_message>
[MOSIP-14369] valid_document xls populated.
</commit_message>
<xml_diff>
--- a/deployment/v3/mosip/kernel/masterdata/upload/xlsx/valid_document.xlsx
+++ b/deployment/v3/mosip/kernel/masterdata/upload/xlsx/valid_document.xlsx
@@ -20,18 +20,129 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="41">
+  <si>
+    <t xml:space="preserve">doctyp_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doccat_code</t>
+  </si>
   <si>
     <t xml:space="preserve">lang_code</t>
   </si>
   <si>
-    <t xml:space="preserve">doctyp_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doccat_code</t>
-  </si>
-  <si>
     <t xml:space="preserve">is_active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOC028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EOP</t>
   </si>
 </sst>
 </file>
@@ -156,15 +267,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3:C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.6"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -181,10 +296,514 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>